<commit_message>
Added routine to handle the blink led pattern command.
</commit_message>
<xml_diff>
--- a/Resources/Commands.xlsx
+++ b/Resources/Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\STM32\Projects\TextualProtocol\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D7C017-5552-4DBC-8EDB-7665028A0B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F4B32D-B36C-44A6-8A16-C5E987D3EF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="39">
   <si>
     <t>Item</t>
   </si>
@@ -103,6 +103,45 @@
   </si>
   <si>
     <t>Enable the echoing of received bytes</t>
+  </si>
+  <si>
+    <t>$blinkpatt,0</t>
+  </si>
+  <si>
+    <t>blinkpatt</t>
+  </si>
+  <si>
+    <t>Blink pattern -&gt; Always off</t>
+  </si>
+  <si>
+    <t>$blinkpatt,1</t>
+  </si>
+  <si>
+    <t>$blinkpatt,2</t>
+  </si>
+  <si>
+    <t>$blinkpatt,3</t>
+  </si>
+  <si>
+    <t>$blinkpatt,4</t>
+  </si>
+  <si>
+    <t>$blinkpatt,5</t>
+  </si>
+  <si>
+    <t>Blink pattern -&gt; Toggle each 100ms</t>
+  </si>
+  <si>
+    <t>Blink pattern -&gt; Short-short-long</t>
+  </si>
+  <si>
+    <t>Blink pattern -&gt; Heart beat</t>
+  </si>
+  <si>
+    <t>Blink pattern -&gt; Toggle each 250ms</t>
+  </si>
+  <si>
+    <t>Blink pattern -&gt; Always on</t>
   </si>
 </sst>
 </file>
@@ -175,10 +214,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -461,16 +500,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB4"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -481,183 +520,501 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="2"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>0</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="4" t="s">
+      <c r="H3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>1</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="4" t="s">
+      <c r="H4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>